<commit_message>
fixed some formatting in the table
</commit_message>
<xml_diff>
--- a/Tables/NaturalRecoveryData.xlsx
+++ b/Tables/NaturalRecoveryData.xlsx
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,6 +204,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -492,13 +493,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:O116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="8.88671875" style="8"/>
     <col min="2" max="2" width="15.44140625" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
@@ -527,7 +528,7 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -583,13 +584,22 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>39</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6">
         <v>0.66666666666666696</v>
       </c>
     </row>
@@ -603,15 +613,24 @@
       <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6">
         <v>0.66666666666666696</v>
       </c>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -623,15 +642,24 @@
       <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6">
         <v>0.63636363636363602</v>
       </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -643,15 +671,24 @@
       <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>64</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6">
         <v>0.609375</v>
       </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -663,15 +700,24 @@
       <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>72</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="K7">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6">
         <v>0.54166666666666696</v>
       </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -683,15 +729,24 @@
       <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6">
         <v>0.52941176470588203</v>
       </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -703,15 +758,24 @@
       <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>99</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
         <v>0.53535353535353503</v>
       </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -723,15 +787,24 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>111</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="H10">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6">
         <v>0.51351351351351304</v>
       </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -743,15 +816,24 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>136</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
         <v>0.20588235294117599</v>
       </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -763,16 +845,25 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>162</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <f>4/224</f>
         <v>1.7857142857142856E-2</v>
       </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -784,15 +875,24 @@
       <c r="C13">
         <v>1936</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>587</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
         <v>0.16695059625212899</v>
       </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -804,13 +904,22 @@
       <c r="C14">
         <v>1955</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>187</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="O14">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6">
         <v>0.72727272727272696</v>
       </c>
     </row>
@@ -824,15 +933,24 @@
       <c r="C15">
         <v>1955</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>192</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
-      <c r="N15">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6">
         <v>0.69270833333333304</v>
       </c>
+      <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -844,15 +962,24 @@
       <c r="C16">
         <v>1955</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>198</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
-      <c r="M16">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6">
         <v>0.66161616161616199</v>
       </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -864,15 +991,24 @@
       <c r="C17">
         <v>1955</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <v>205</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
       </c>
-      <c r="L17">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6">
         <v>0.62926829268292706</v>
       </c>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -884,15 +1020,24 @@
       <c r="C18">
         <v>1955</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>215</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
       </c>
-      <c r="K18">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6">
         <v>0.61395348837209296</v>
       </c>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -904,15 +1049,24 @@
       <c r="C19">
         <v>1955</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <v>228</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
       </c>
-      <c r="J19">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6">
         <v>0.54824561403508798</v>
       </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -924,15 +1078,24 @@
       <c r="C20">
         <v>1955</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <v>240</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
       </c>
-      <c r="I20">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6">
         <v>0.42916666666666697</v>
       </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -944,15 +1107,24 @@
       <c r="C21">
         <v>1955</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="5">
         <v>259</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6">
         <v>0.28185328185328201</v>
       </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -964,15 +1136,24 @@
       <c r="C22">
         <v>1955</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="5">
         <v>271</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="G22">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6">
         <v>0.107011070110701</v>
       </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -984,15 +1165,24 @@
       <c r="C23">
         <v>1955</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="5">
         <v>298</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -1004,13 +1194,22 @@
       <c r="C24">
         <v>1941</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="5">
         <v>113.70370370370399</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="O24">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6">
         <v>0.33420195439739397</v>
       </c>
     </row>
@@ -1024,15 +1223,24 @@
       <c r="C25">
         <v>1941</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="5">
         <v>135</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="J25">
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6">
         <v>0.38518518518518502</v>
       </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -1044,15 +1252,24 @@
       <c r="C26">
         <v>1941</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="5">
         <v>192</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="H26">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6">
         <v>0.24479166666666699</v>
       </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -1064,13 +1281,22 @@
       <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="5">
         <v>72</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
-      <c r="O27">
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6">
         <v>0.69444444444444398</v>
       </c>
     </row>
@@ -1084,15 +1310,24 @@
       <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="5">
         <v>85</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
-      <c r="N28">
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6">
         <v>0.70588235294117696</v>
       </c>
+      <c r="O28" s="6"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -1104,15 +1339,24 @@
       <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="5">
         <v>102</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="M29">
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6">
         <v>0.69607843137254899</v>
       </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -1124,15 +1368,24 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="5">
         <v>116</v>
       </c>
       <c r="E30" t="s">
         <v>3</v>
       </c>
-      <c r="L30">
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6">
         <v>0.73275862068965503</v>
       </c>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -1144,15 +1397,24 @@
       <c r="C31" t="s">
         <v>39</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="5">
         <v>138</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
       </c>
-      <c r="K31">
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6">
         <v>0.64492753623188404</v>
       </c>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -1164,15 +1426,24 @@
       <c r="C32" t="s">
         <v>39</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="5">
         <v>164</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
       </c>
-      <c r="J32">
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6">
         <v>0.60975609756097604</v>
       </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -1184,15 +1455,24 @@
       <c r="C33" t="s">
         <v>39</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="5">
         <v>178</v>
       </c>
       <c r="E33" t="s">
         <v>3</v>
       </c>
-      <c r="I33">
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6">
         <v>0.62359550561797705</v>
       </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -1204,15 +1484,24 @@
       <c r="C34" t="s">
         <v>39</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="5">
         <v>188</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
       </c>
-      <c r="H34">
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6">
         <v>0.52659574468085102</v>
       </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -1224,15 +1513,24 @@
       <c r="C35" t="s">
         <v>39</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="5">
         <v>200</v>
       </c>
       <c r="E35" t="s">
         <v>3</v>
       </c>
-      <c r="G35">
+      <c r="F35" s="6"/>
+      <c r="G35" s="6">
         <v>0.41499999999999998</v>
       </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1244,15 +1542,24 @@
       <c r="C36" t="s">
         <v>39</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="5">
         <v>211</v>
       </c>
       <c r="E36" t="s">
         <v>3</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="6">
         <v>3.3175355450236997E-2</v>
       </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -1264,15 +1571,24 @@
       <c r="C37">
         <v>1936</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="5">
         <v>155</v>
       </c>
       <c r="E37" t="s">
         <v>3</v>
       </c>
-      <c r="I37">
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6">
         <v>0.40645161290322601</v>
       </c>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -1284,13 +1600,22 @@
       <c r="C38">
         <v>1955</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="5">
         <v>972</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
       </c>
-      <c r="O38">
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6">
         <v>0.86625514403292203</v>
       </c>
     </row>
@@ -1304,15 +1629,24 @@
       <c r="C39">
         <v>1955</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="5">
         <v>995</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
       </c>
-      <c r="N39">
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6">
         <v>0.85527638190954802</v>
       </c>
+      <c r="O39" s="6"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -1324,15 +1658,24 @@
       <c r="C40">
         <v>1955</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="5">
         <v>1022</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
       </c>
-      <c r="M40">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6">
         <v>0.82583170254403104</v>
       </c>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -1344,15 +1687,24 @@
       <c r="C41">
         <v>1955</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="5">
         <v>1044</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
       </c>
-      <c r="L41">
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6">
         <v>0.79406130268199204</v>
       </c>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -1364,15 +1716,24 @@
       <c r="C42">
         <v>1955</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="5">
         <v>1071</v>
       </c>
       <c r="E42" t="s">
         <v>3</v>
       </c>
-      <c r="K42">
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6">
         <v>0.75910364145658304</v>
       </c>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -1384,15 +1745,24 @@
       <c r="C43">
         <v>1955</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="5">
         <v>1093</v>
       </c>
       <c r="E43" t="s">
         <v>3</v>
       </c>
-      <c r="J43">
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6">
         <v>0.722781335773102</v>
       </c>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -1404,15 +1774,24 @@
       <c r="C44">
         <v>1955</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="5">
         <v>1121</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
       </c>
-      <c r="I44">
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6">
         <v>0.66547725245316702</v>
       </c>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -1424,15 +1803,24 @@
       <c r="C45">
         <v>1955</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="5">
         <v>1145</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
       </c>
-      <c r="H45">
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6">
         <v>0.55807860262008702</v>
       </c>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -1444,15 +1832,24 @@
       <c r="C46">
         <v>1955</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="5">
         <v>1185</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
       </c>
-      <c r="G46">
+      <c r="F46" s="6"/>
+      <c r="G46" s="6">
         <v>0.353586497890295</v>
       </c>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -1464,15 +1861,24 @@
       <c r="C47">
         <v>1955</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="5">
         <v>1206</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
+      <c r="F47" s="6">
+        <v>0</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -1484,13 +1890,22 @@
       <c r="C48">
         <v>1941</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="5">
         <v>346.56793661496999</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
       </c>
-      <c r="O48">
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6">
         <v>0.43858644710364297</v>
       </c>
     </row>
@@ -1504,15 +1919,24 @@
       <c r="C49">
         <v>1941</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="5">
         <v>414.46288209607002</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
       </c>
-      <c r="J49">
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6">
         <v>0.57182442683749202</v>
       </c>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -1524,15 +1948,24 @@
       <c r="C50">
         <v>1941</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="5">
         <v>458</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
       </c>
-      <c r="H50">
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6">
         <v>0.49563318777292598</v>
       </c>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -1544,13 +1977,22 @@
       <c r="C51" t="s">
         <v>39</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="5">
         <v>128</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
       </c>
-      <c r="O51">
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6">
         <v>0.609375</v>
       </c>
     </row>
@@ -1564,15 +2006,24 @@
       <c r="C52" t="s">
         <v>39</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="5">
         <v>158</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
       </c>
-      <c r="N52">
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6">
         <v>0.626582278481013</v>
       </c>
+      <c r="O52" s="6"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -1584,15 +2035,24 @@
       <c r="C53" t="s">
         <v>39</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="5">
         <v>217</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
       </c>
-      <c r="M53">
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6">
         <v>0.55760368663594495</v>
       </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -1604,15 +2064,24 @@
       <c r="C54" t="s">
         <v>39</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="5">
         <v>263</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
       </c>
-      <c r="L54">
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6">
         <v>0.62737642585551301</v>
       </c>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -1624,15 +2093,24 @@
       <c r="C55" t="s">
         <v>39</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="5">
         <v>300</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
       </c>
-      <c r="K55">
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6">
         <v>0.67</v>
       </c>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -1644,15 +2122,24 @@
       <c r="C56" t="s">
         <v>39</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="5">
         <v>365</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
       </c>
-      <c r="J56">
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6">
         <v>0.63287671232876697</v>
       </c>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -1664,15 +2151,24 @@
       <c r="C57" t="s">
         <v>39</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="5">
         <v>426</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
       </c>
-      <c r="I57">
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6">
         <v>0.67840375586854496</v>
       </c>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -1684,15 +2180,24 @@
       <c r="C58" t="s">
         <v>39</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="5">
         <v>439</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
       </c>
-      <c r="H58">
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6">
         <v>0.79498861047836</v>
       </c>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -1704,15 +2209,24 @@
       <c r="C59" t="s">
         <v>39</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="5">
         <v>447</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
       </c>
-      <c r="G59">
+      <c r="F59" s="6"/>
+      <c r="G59" s="6">
         <v>0.79194630872483196</v>
       </c>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -1724,15 +2238,24 @@
       <c r="C60" t="s">
         <v>39</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="5">
         <v>448</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="6">
         <v>0.765625</v>
       </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -1744,15 +2267,24 @@
       <c r="C61">
         <v>1936</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="5">
         <v>4</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
       </c>
-      <c r="I61">
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6">
         <v>0.75</v>
       </c>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -1764,13 +2296,22 @@
       <c r="C62">
         <v>1941</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="5">
         <v>272.30210051688101</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
       </c>
-      <c r="O62">
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="6">
         <v>0.50679006786231096</v>
       </c>
     </row>
@@ -1784,15 +2325,24 @@
       <c r="C63">
         <v>1941</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="5">
         <v>326.69461077844301</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
       </c>
-      <c r="J63">
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6">
         <v>0.74993584808827296</v>
       </c>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -1804,15 +2354,24 @@
       <c r="C64">
         <v>1941</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="5">
         <v>334</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
       </c>
-      <c r="H64">
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6">
         <v>0.80239520958083799</v>
       </c>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -1824,15 +2383,24 @@
       <c r="C65">
         <v>1939</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="5">
         <v>247</v>
       </c>
       <c r="E65" t="s">
         <v>16</v>
       </c>
-      <c r="G65">
+      <c r="F65" s="6"/>
+      <c r="G65" s="6">
         <v>0.55870445344129605</v>
       </c>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -1844,21 +2412,28 @@
       <c r="C66">
         <v>1939</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="5">
         <v>259</v>
       </c>
       <c r="E66" t="s">
         <v>16</v>
       </c>
-      <c r="G66">
+      <c r="F66" s="6"/>
+      <c r="G66" s="6">
         <v>0.38996138996139001</v>
       </c>
-      <c r="I66">
+      <c r="H66" s="6"/>
+      <c r="I66" s="6">
         <v>0.40154440154440202</v>
       </c>
-      <c r="K66">
+      <c r="J66" s="6"/>
+      <c r="K66" s="6">
         <v>0.37837837837837801</v>
       </c>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
@@ -1870,25 +2445,30 @@
       <c r="C67">
         <v>1939</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="5">
         <v>280</v>
       </c>
       <c r="E67" t="s">
         <v>16</v>
       </c>
-      <c r="G67">
+      <c r="F67" s="6"/>
+      <c r="G67" s="6">
         <v>0.36071428571428599</v>
       </c>
-      <c r="I67">
+      <c r="H67" s="6"/>
+      <c r="I67" s="6">
         <v>0.32142857142857101</v>
       </c>
-      <c r="K67">
+      <c r="J67" s="6"/>
+      <c r="K67" s="6">
         <v>0.310714285714286</v>
       </c>
-      <c r="M67">
+      <c r="L67" s="6"/>
+      <c r="M67" s="6">
         <v>0.3</v>
       </c>
-      <c r="O67">
+      <c r="N67" s="6"/>
+      <c r="O67" s="6">
         <v>0.28928571428571398</v>
       </c>
     </row>
@@ -1902,18 +2482,26 @@
       <c r="C68">
         <v>1939</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="5">
         <v>345</v>
       </c>
       <c r="E68" t="s">
         <v>16</v>
       </c>
-      <c r="G68">
+      <c r="F68" s="6"/>
+      <c r="G68" s="6">
         <v>0.46086956521739098</v>
       </c>
-      <c r="I68">
+      <c r="H68" s="6"/>
+      <c r="I68" s="6">
         <v>0.46086956521739098</v>
       </c>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -1925,15 +2513,24 @@
       <c r="C69">
         <v>1939</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="5">
         <v>171</v>
       </c>
       <c r="E69" t="s">
         <v>14</v>
       </c>
-      <c r="G69">
+      <c r="F69" s="6"/>
+      <c r="G69" s="6">
         <v>0.77192982456140302</v>
       </c>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
@@ -1945,18 +2542,26 @@
       <c r="C70">
         <v>1939</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="5">
         <v>479</v>
       </c>
       <c r="E70" t="s">
         <v>14</v>
       </c>
-      <c r="G70">
+      <c r="F70" s="6"/>
+      <c r="G70" s="6">
         <v>0.78079331941544905</v>
       </c>
-      <c r="I70">
+      <c r="H70" s="6"/>
+      <c r="I70" s="6">
         <v>0.73903966597077198</v>
       </c>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -1968,21 +2573,28 @@
       <c r="C71">
         <v>1939</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="5">
         <v>849</v>
       </c>
       <c r="E71" t="s">
         <v>14</v>
       </c>
-      <c r="G71">
+      <c r="F71" s="6"/>
+      <c r="G71" s="6">
         <v>0.73027090694935204</v>
       </c>
-      <c r="I71">
+      <c r="H71" s="6"/>
+      <c r="I71" s="6">
         <v>0.77031802120141302</v>
       </c>
-      <c r="K71">
+      <c r="J71" s="6"/>
+      <c r="K71" s="6">
         <v>0.73027090694935204</v>
       </c>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -1994,25 +2606,30 @@
       <c r="C72">
         <v>1939</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="5">
         <v>985</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
       </c>
-      <c r="G72">
+      <c r="F72" s="6"/>
+      <c r="G72" s="6">
         <v>0.70964467005076104</v>
       </c>
-      <c r="I72">
+      <c r="H72" s="6"/>
+      <c r="I72" s="6">
         <v>0.70964467005076104</v>
       </c>
-      <c r="K72">
+      <c r="J72" s="6"/>
+      <c r="K72" s="6">
         <v>0.70050761421319796</v>
       </c>
-      <c r="M72">
+      <c r="L72" s="6"/>
+      <c r="M72" s="6">
         <v>0.71979695431472102</v>
       </c>
-      <c r="O72">
+      <c r="N72" s="6"/>
+      <c r="O72" s="6">
         <v>0.69035532994923898</v>
       </c>
     </row>
@@ -2026,15 +2643,24 @@
       <c r="C73">
         <v>1954</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="5">
         <v>879</v>
       </c>
       <c r="E73" t="s">
         <v>0</v>
       </c>
-      <c r="L73">
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6">
         <v>0.86575654152446002</v>
       </c>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -2046,12 +2672,22 @@
       <c r="C74">
         <v>1954</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="5">
         <v>899</v>
       </c>
       <c r="E74" t="s">
         <v>0</v>
       </c>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75">
@@ -2063,15 +2699,24 @@
       <c r="C75">
         <v>1926</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="5">
         <v>1953</v>
       </c>
       <c r="E75" t="s">
         <v>0</v>
       </c>
-      <c r="L75">
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6">
         <v>0.39016897081413199</v>
       </c>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -2083,13 +2728,22 @@
       <c r="C76">
         <v>1906</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="5">
         <v>1627</v>
       </c>
       <c r="E76" t="s">
         <v>0</v>
       </c>
-      <c r="O76">
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6">
         <v>0.11001843884449899</v>
       </c>
     </row>
@@ -2103,15 +2757,24 @@
       <c r="C77">
         <v>1906</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="5">
         <v>1658</v>
       </c>
       <c r="E77" t="s">
         <v>0</v>
       </c>
-      <c r="N77">
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6">
         <v>0.13088057901085601</v>
       </c>
+      <c r="O77" s="6"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -2123,15 +2786,24 @@
       <c r="C78">
         <v>1906</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="5">
         <v>1731</v>
       </c>
       <c r="E78" t="s">
         <v>0</v>
       </c>
-      <c r="M78">
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6">
         <v>0.16002310803004</v>
       </c>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -2143,15 +2815,24 @@
       <c r="C79">
         <v>1906</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="5">
         <v>1804</v>
       </c>
       <c r="E79" t="s">
         <v>0</v>
       </c>
-      <c r="L79">
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6">
         <v>0.18403547671840401</v>
       </c>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
@@ -2163,17 +2844,26 @@
       <c r="C80">
         <v>1906</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="5">
         <v>1872</v>
       </c>
       <c r="E80" t="s">
         <v>0</v>
       </c>
-      <c r="K80">
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6">
         <v>0.206730769230769</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -2183,17 +2873,26 @@
       <c r="C81">
         <v>1906</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="5">
         <v>1949</v>
       </c>
       <c r="E81" t="s">
         <v>0</v>
       </c>
-      <c r="J81">
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6">
         <v>0.23242688558235</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -2203,17 +2902,26 @@
       <c r="C82">
         <v>1906</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="5">
         <v>2022</v>
       </c>
       <c r="E82" t="s">
         <v>0</v>
       </c>
-      <c r="I82">
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6">
         <v>0.23491592482690399</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -2223,17 +2931,26 @@
       <c r="C83">
         <v>1933</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="5">
         <v>637</v>
       </c>
       <c r="E83" t="s">
         <v>0</v>
       </c>
-      <c r="N83">
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6">
         <v>0.420722135007849</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O83" s="6"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2243,17 +2960,26 @@
       <c r="C84">
         <v>1933</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="5">
         <v>747</v>
       </c>
       <c r="E84" t="s">
         <v>0</v>
       </c>
-      <c r="J84">
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6">
         <v>0.50468540829986597</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2263,17 +2989,26 @@
       <c r="C85">
         <v>1933</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="5">
         <v>1150</v>
       </c>
       <c r="E85" t="s">
         <v>0</v>
       </c>
-      <c r="G85">
+      <c r="F85" s="6"/>
+      <c r="G85" s="6">
         <v>0.48260869565217401</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -2283,17 +3018,26 @@
       <c r="C86">
         <v>1933</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="5">
         <v>1189</v>
       </c>
       <c r="E86" t="s">
         <v>0</v>
       </c>
-      <c r="M86">
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6">
         <v>0.455004205214466</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2303,17 +3047,26 @@
       <c r="C87">
         <v>1933</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="5">
         <v>1195</v>
       </c>
       <c r="E87" t="s">
         <v>0</v>
       </c>
-      <c r="K87">
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6">
         <v>0.40502092050209199</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -2323,17 +3076,26 @@
       <c r="C88">
         <v>1933</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="5">
         <v>1308</v>
       </c>
       <c r="E88" t="s">
         <v>0</v>
       </c>
-      <c r="L88">
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6">
         <v>0.39984709480122299</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+      <c r="O88" s="6"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2343,17 +3105,26 @@
       <c r="C89">
         <v>1933</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="5">
         <v>1309</v>
       </c>
       <c r="E89" t="s">
         <v>0</v>
       </c>
-      <c r="H89">
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6">
         <v>0.48663101604278097</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
+      <c r="O89" s="6"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -2363,17 +3134,26 @@
       <c r="C90">
         <v>1933</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="5">
         <v>1603</v>
       </c>
       <c r="E90" t="s">
         <v>0</v>
       </c>
-      <c r="I90">
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6">
         <v>0.51029320024953195</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="O90" s="6"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>12</v>
       </c>
@@ -2383,17 +3163,26 @@
       <c r="C91">
         <v>1974</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="5">
         <v>40</v>
       </c>
       <c r="E91" t="s">
         <v>0</v>
       </c>
-      <c r="G91">
+      <c r="F91" s="6"/>
+      <c r="G91" s="6">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="6"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>12</v>
       </c>
@@ -2403,17 +3192,26 @@
       <c r="C92">
         <v>1974</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="5">
         <v>70</v>
       </c>
       <c r="E92" t="s">
         <v>0</v>
       </c>
-      <c r="G92">
+      <c r="F92" s="6"/>
+      <c r="G92" s="6">
         <v>0.47142857142857097</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>12</v>
       </c>
@@ -2423,17 +3221,26 @@
       <c r="C93">
         <v>1974</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="5">
         <v>75</v>
       </c>
       <c r="E93" t="s">
         <v>0</v>
       </c>
-      <c r="J93">
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6">
         <v>0.54666666666666697</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>12</v>
       </c>
@@ -2443,17 +3250,26 @@
       <c r="C94">
         <v>1974</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="5">
         <v>88</v>
       </c>
       <c r="E94" t="s">
         <v>0</v>
       </c>
-      <c r="H94">
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>12</v>
       </c>
@@ -2463,17 +3279,26 @@
       <c r="C95">
         <v>1974</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="5">
         <v>119</v>
       </c>
       <c r="E95" t="s">
         <v>0</v>
       </c>
-      <c r="G95">
+      <c r="F95" s="6"/>
+      <c r="G95" s="6">
         <v>0.24369747899159699</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>12</v>
       </c>
@@ -2483,15 +3308,24 @@
       <c r="C96">
         <v>1974</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="5">
         <v>126</v>
       </c>
       <c r="E96" t="s">
         <v>0</v>
       </c>
-      <c r="G96">
+      <c r="F96" s="6"/>
+      <c r="G96" s="6">
         <v>0.27777777777777801</v>
       </c>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97">
@@ -2503,15 +3337,24 @@
       <c r="C97">
         <v>1974</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="5">
         <v>136</v>
       </c>
       <c r="E97" t="s">
         <v>0</v>
       </c>
-      <c r="G97">
+      <c r="F97" s="6"/>
+      <c r="G97" s="6">
         <v>0.38970588235294101</v>
       </c>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
+      <c r="O97" s="6"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98">
@@ -2523,15 +3366,24 @@
       <c r="C98">
         <v>1974</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="5">
         <v>154</v>
       </c>
       <c r="E98" t="s">
         <v>0</v>
       </c>
-      <c r="G98">
+      <c r="F98" s="6"/>
+      <c r="G98" s="6">
         <v>0.32467532467532501</v>
       </c>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+      <c r="O98" s="6"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99">
@@ -2543,15 +3395,24 @@
       <c r="C99">
         <v>1971</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="5">
         <v>571</v>
       </c>
       <c r="E99" t="s">
         <v>0</v>
       </c>
-      <c r="I99">
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6">
         <v>0.25744308231173402</v>
       </c>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
+      <c r="O99" s="6"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
@@ -2563,15 +3424,24 @@
       <c r="C100">
         <v>1903</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="5">
         <v>243</v>
       </c>
       <c r="E100" t="s">
         <v>0</v>
       </c>
-      <c r="N100">
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6">
         <v>0.13580246913580199</v>
       </c>
+      <c r="O100" s="6"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
@@ -2583,15 +3453,24 @@
       <c r="C101">
         <v>1903</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="5">
         <v>277</v>
       </c>
       <c r="E101" t="s">
         <v>0</v>
       </c>
-      <c r="M101">
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6">
         <v>0.20577617328519901</v>
       </c>
+      <c r="N101" s="6"/>
+      <c r="O101" s="6"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
@@ -2603,15 +3482,24 @@
       <c r="C102">
         <v>1903</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="5">
         <v>311</v>
       </c>
       <c r="E102" t="s">
         <v>0</v>
       </c>
-      <c r="L102">
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6">
         <v>0.25401929260450201</v>
       </c>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
@@ -2623,15 +3511,24 @@
       <c r="C103">
         <v>1903</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="5">
         <v>357</v>
       </c>
       <c r="E103" t="s">
         <v>0</v>
       </c>
-      <c r="K103">
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6">
         <v>0.31932773109243701</v>
       </c>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
+      <c r="O103" s="6"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
@@ -2643,15 +3540,24 @@
       <c r="C104">
         <v>1903</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="5">
         <v>397</v>
       </c>
       <c r="E104" t="s">
         <v>0</v>
       </c>
-      <c r="J104">
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6">
         <v>0.36020151133501299</v>
       </c>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="6"/>
+      <c r="O104" s="6"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
@@ -2663,15 +3569,24 @@
       <c r="C105">
         <v>1903</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="5">
         <v>448</v>
       </c>
       <c r="E105" t="s">
         <v>0</v>
       </c>
-      <c r="I105">
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6">
         <v>0.39732142857142899</v>
       </c>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
@@ -2683,15 +3598,24 @@
       <c r="C106">
         <v>1903</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="5">
         <v>477</v>
       </c>
       <c r="E106" t="s">
         <v>0</v>
       </c>
-      <c r="H106">
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6">
         <v>0.41509433962264197</v>
       </c>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
@@ -2703,15 +3627,24 @@
       <c r="C107">
         <v>1903</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="5">
         <v>541</v>
       </c>
       <c r="E107" t="s">
         <v>0</v>
       </c>
-      <c r="G107">
+      <c r="F107" s="6"/>
+      <c r="G107" s="6">
         <v>0.46580406654343798</v>
       </c>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
+      <c r="O107" s="6"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
@@ -2723,15 +3656,24 @@
       <c r="C108">
         <v>1903</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="5">
         <v>670</v>
       </c>
       <c r="E108" t="s">
         <v>0</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="6">
         <v>0.55074626865671605</v>
       </c>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109">
@@ -2743,15 +3685,24 @@
       <c r="C109">
         <v>1935</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="5">
         <v>158</v>
       </c>
       <c r="E109" t="s">
         <v>0</v>
       </c>
-      <c r="M109">
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="6">
         <v>0.278481012658228</v>
       </c>
+      <c r="N109" s="6"/>
+      <c r="O109" s="6"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110">
@@ -2763,13 +3714,22 @@
       <c r="C110">
         <v>1935</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="5">
         <v>171</v>
       </c>
       <c r="E110" t="s">
         <v>0</v>
       </c>
-      <c r="O110">
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="6"/>
+      <c r="O110" s="6">
         <v>0.25730994152046799</v>
       </c>
     </row>
@@ -2783,15 +3743,24 @@
       <c r="C111">
         <v>1935</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="5">
         <v>183</v>
       </c>
       <c r="E111" t="s">
         <v>0</v>
       </c>
-      <c r="N111">
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
+      <c r="N111" s="6">
         <v>0.29508196721311503</v>
       </c>
+      <c r="O111" s="6"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112">
@@ -2803,17 +3772,26 @@
       <c r="C112">
         <v>1935</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="5">
         <v>214</v>
       </c>
       <c r="E112" t="s">
         <v>0</v>
       </c>
-      <c r="L112">
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="6">
         <v>0.26635514018691597</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M112" s="6"/>
+      <c r="N112" s="6"/>
+      <c r="O112" s="6"/>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>91</v>
       </c>
@@ -2823,17 +3801,26 @@
       <c r="C113">
         <v>1935</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="5">
         <v>232</v>
       </c>
       <c r="E113" t="s">
         <v>0</v>
       </c>
-      <c r="J113">
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6">
         <v>0.31034482758620702</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="6"/>
+      <c r="O113" s="6"/>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>91</v>
       </c>
@@ -2843,17 +3830,26 @@
       <c r="C114">
         <v>1935</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="5">
         <v>239</v>
       </c>
       <c r="E114" t="s">
         <v>0</v>
       </c>
-      <c r="K114">
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6">
         <v>0.330543933054393</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
+      <c r="N114" s="6"/>
+      <c r="O114" s="6"/>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>91</v>
       </c>
@@ -2863,17 +3859,26 @@
       <c r="C115">
         <v>1935</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="5">
         <v>266</v>
       </c>
       <c r="E115" t="s">
         <v>0</v>
       </c>
-      <c r="I115">
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6">
         <v>0.27443609022556398</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+      <c r="N115" s="6"/>
+      <c r="O115" s="6"/>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>91</v>
       </c>
@@ -2883,15 +3888,24 @@
       <c r="C116">
         <v>1935</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="5">
         <v>362</v>
       </c>
       <c r="E116" t="s">
         <v>0</v>
       </c>
-      <c r="H116">
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6">
         <v>0.25414364640884002</v>
       </c>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
+      <c r="N116" s="6"/>
+      <c r="O116" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A3:O87">
@@ -2923,7 +3937,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
+      <c r="A1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>

</xml_diff>